<commit_message>
hierrachy and new forms
</commit_message>
<xml_diff>
--- a/forms/app/cholera_suspicion_follow_up.xlsx
+++ b/forms/app/cholera_suspicion_follow_up.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -268,7 +268,7 @@
     <t xml:space="preserve">danger_signs</t>
   </si>
   <si>
-    <t xml:space="preserve">Danger Sign Follow-up - Baby</t>
+    <t xml:space="preserve">Cholera Follow Up Form</t>
   </si>
   <si>
     <t xml:space="preserve">select_one yes_no</t>
@@ -1300,15 +1300,15 @@
   </sheetPr>
   <dimension ref="A1:AJ72"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="J49" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="J1" activeCellId="0" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="A49" activeCellId="0" sqref="A49"/>
-      <selection pane="bottomRight" activeCell="U57" activeCellId="0" sqref="U57"/>
+      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="bottomRight" activeCell="C33" activeCellId="0" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.29"/>
@@ -1323,7 +1323,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="32.71"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="20" min="15" style="0" width="25.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="73.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="30.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="30.02"/>
     <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="29" min="24" style="0" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="31" style="0" width="29.86"/>
   </cols>
@@ -4632,7 +4632,7 @@
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="2" style="0" width="45.86"/>
@@ -4971,15 +4971,15 @@
   </sheetPr>
   <dimension ref="A1:Z2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.57"/>
   </cols>
@@ -5035,7 +5035,7 @@
       </c>
       <c r="C2" s="27" t="n">
         <f aca="true">NOW()</f>
-        <v>45241.8320923893</v>
+        <v>45245.7854186156</v>
       </c>
       <c r="D2" s="23" t="s">
         <v>188</v>
@@ -5091,7 +5091,7 @@
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="2" style="0" width="45.86"/>

</xml_diff>

<commit_message>
configured cha to verify case from chp
</commit_message>
<xml_diff>
--- a/forms/app/cholera_suspicion_follow_up.xlsx
+++ b/forms/app/cholera_suspicion_follow_up.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -543,6 +543,7 @@
         <color rgb="FF000000"/>
         <rFont val="Cambria"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">profuse_watery_diarrhea</t>
     </r>
@@ -577,6 +578,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">dehydration</t>
     </r>
@@ -871,7 +873,7 @@
     <t xml:space="preserve">Cholera Suspicion Follow Up</t>
   </si>
   <si>
-    <t xml:space="preserve">cholera_follow_up</t>
+    <t xml:space="preserve">cholera_suspicion_follow_up</t>
   </si>
   <si>
     <t xml:space="preserve">pages</t>
@@ -1182,7 +1184,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd\-mm\-yyyy\ hh\-mm\-ss"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1238,18 +1240,6 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Cambria"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1483,43 +1473,51 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="15" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="15" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1527,27 +1525,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="16" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="16" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1630,7 +1620,7 @@
   </sheetPr>
   <dimension ref="A1:AJ81"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="K36" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="K1" activeCellId="0" sqref="K1"/>
@@ -1638,7 +1628,7 @@
       <selection pane="bottomRight" activeCell="K59" activeCellId="0" sqref="K59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.29"/>
@@ -5226,7 +5216,7 @@
       <selection pane="bottomLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="2" style="0" width="45.86"/>
@@ -5627,13 +5617,13 @@
   </sheetPr>
   <dimension ref="A1:Z2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.7"/>
@@ -5691,7 +5681,7 @@
       </c>
       <c r="C2" s="32" t="n">
         <f aca="true">NOW()</f>
-        <v>45261.382722172</v>
+        <v>45266.4253990188</v>
       </c>
       <c r="D2" s="29" t="s">
         <v>171</v>
@@ -5747,7 +5737,7 @@
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="2" style="0" width="45.86"/>

</xml_diff>

<commit_message>
added and uploaded improved forms
</commit_message>
<xml_diff>
--- a/forms/app/cholera_suspicion_follow_up.xlsx
+++ b/forms/app/cholera_suspicion_follow_up.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="273">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -802,6 +802,12 @@
       </rPr>
       <t xml:space="preserve">} = 'yes'</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">the_finding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Findings &lt;i class="fa fa-medkit" aria-hidden="true"&gt;&lt;/i&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">advise</t>
@@ -1621,14 +1627,14 @@
   <dimension ref="A1:AJ81"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="K36" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C42" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="K1" activeCellId="0" sqref="K1"/>
-      <selection pane="bottomLeft" activeCell="A36" activeCellId="0" sqref="A36"/>
-      <selection pane="bottomRight" activeCell="K59" activeCellId="0" sqref="K59"/>
+      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A42" activeCellId="0" sqref="A42"/>
+      <selection pane="bottomRight" activeCell="L66" activeCellId="0" sqref="L66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.29"/>
@@ -4537,9 +4543,15 @@
       <c r="AJ65" s="14"/>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A66" s="16"/>
-      <c r="B66" s="16"/>
-      <c r="C66" s="4"/>
+      <c r="A66" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B66" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="C66" s="13" t="s">
+        <v>148</v>
+      </c>
       <c r="D66" s="14"/>
       <c r="E66" s="14"/>
       <c r="F66" s="14"/>
@@ -4547,8 +4559,12 @@
       <c r="H66" s="14"/>
       <c r="I66" s="14"/>
       <c r="J66" s="14"/>
-      <c r="K66" s="9"/>
-      <c r="L66" s="12"/>
+      <c r="K66" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="L66" s="12" t="s">
+        <v>122</v>
+      </c>
       <c r="M66" s="14"/>
       <c r="N66" s="14"/>
       <c r="O66" s="14"/>
@@ -4579,10 +4595,10 @@
         <v>89</v>
       </c>
       <c r="B67" s="16" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C67" s="13" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D67" s="14"/>
       <c r="E67" s="14"/>
@@ -4627,10 +4643,10 @@
         <v>89</v>
       </c>
       <c r="B68" s="17" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C68" s="13" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D68" s="14"/>
       <c r="E68" s="14"/>
@@ -4643,7 +4659,7 @@
         <v>92</v>
       </c>
       <c r="L68" s="12" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="M68" s="14"/>
       <c r="N68" s="14"/>
@@ -4675,10 +4691,10 @@
         <v>89</v>
       </c>
       <c r="B69" s="17" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C69" s="13" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D69" s="14"/>
       <c r="E69" s="14"/>
@@ -4723,10 +4739,10 @@
         <v>89</v>
       </c>
       <c r="B70" s="17" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C70" s="13" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D70" s="14"/>
       <c r="E70" s="14"/>
@@ -5216,7 +5232,7 @@
       <selection pane="bottomLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="2" style="0" width="45.86"/>
@@ -5224,7 +5240,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="20" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B1" s="20" t="s">
         <v>1</v>
@@ -5266,13 +5282,13 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="28" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B2" s="28" t="s">
         <v>81</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
@@ -5296,13 +5312,13 @@
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="28" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10"/>
@@ -5326,7 +5342,7 @@
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="28" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>93</v>
@@ -5356,7 +5372,7 @@
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="28" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>95</v>
@@ -5367,7 +5383,7 @@
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="28" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>97</v>
@@ -5378,7 +5394,7 @@
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="28" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>99</v>
@@ -5389,7 +5405,7 @@
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="28" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>101</v>
@@ -5400,7 +5416,7 @@
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="28" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>103</v>
@@ -5411,7 +5427,7 @@
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="28" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>105</v>
@@ -5422,7 +5438,7 @@
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="28" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>107</v>
@@ -5623,7 +5639,7 @@
       <selection pane="bottomLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.7"/>
@@ -5632,25 +5648,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="20" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="F1" s="20" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="G1" s="30" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H1" s="20"/>
       <c r="I1" s="20"/>
@@ -5674,24 +5690,24 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="31" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C2" s="32" t="n">
         <f aca="true">NOW()</f>
-        <v>45266.4253990188</v>
+        <v>45273.7085153842</v>
       </c>
       <c r="D2" s="29" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E2" s="29" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="F2" s="28"/>
       <c r="G2" s="33" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H2" s="28"/>
       <c r="I2" s="28"/>
@@ -5737,7 +5753,7 @@
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="2" style="0" width="45.86"/>
@@ -5745,7 +5761,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="20" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B1" s="20" t="s">
         <v>1</v>
@@ -5788,13 +5804,13 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>81</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
@@ -5819,13 +5835,13 @@
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10"/>
@@ -5875,13 +5891,13 @@
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
@@ -5906,13 +5922,13 @@
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
@@ -5937,13 +5953,13 @@
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
@@ -5968,13 +5984,13 @@
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="10" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
@@ -5999,13 +6015,13 @@
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="10" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
@@ -6055,13 +6071,13 @@
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="10" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
@@ -6086,13 +6102,13 @@
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="10" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
@@ -6117,13 +6133,13 @@
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="10" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
@@ -6148,13 +6164,13 @@
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="10" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
@@ -6179,13 +6195,13 @@
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="10" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
@@ -6210,13 +6226,13 @@
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="10" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
@@ -6266,13 +6282,13 @@
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="10" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
@@ -6297,13 +6313,13 @@
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="10" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
@@ -6328,13 +6344,13 @@
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="10" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
@@ -6359,13 +6375,13 @@
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="10" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
@@ -6390,13 +6406,13 @@
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="B22" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="B22" s="10" t="s">
-        <v>196</v>
-      </c>
       <c r="C22" s="10" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
@@ -6421,13 +6437,13 @@
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="10" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
@@ -6477,13 +6493,13 @@
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="10" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
@@ -6508,13 +6524,13 @@
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="10" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
@@ -6539,13 +6555,13 @@
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="10" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
@@ -6570,13 +6586,13 @@
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="10" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
@@ -6601,13 +6617,13 @@
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="10" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
@@ -6657,13 +6673,13 @@
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="10" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D31" s="10"/>
       <c r="E31" s="10"/>
@@ -6688,13 +6704,13 @@
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="10" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D32" s="10"/>
       <c r="E32" s="10"/>
@@ -6744,121 +6760,121 @@
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B34" s="0" t="str">
         <f aca="false">SUBSTITUTE(LOWER(SUBSTITUTE(SUBSTITUTE(C34, "(", ""), ")", "")), " ", "_")</f>
         <v>combined_oral_contraceptives</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B35" s="0" t="str">
         <f aca="false">SUBSTITUTE(LOWER(SUBSTITUTE(SUBSTITUTE(C35, "(", ""), ")", "")), " ", "_")</f>
         <v>progesterone_only_pills</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B36" s="0" t="str">
         <f aca="false">SUBSTITUTE(LOWER(SUBSTITUTE(SUBSTITUTE(C36, "(", ""), ")", "")), " ", "_")</f>
         <v>injectibles</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B37" s="0" t="str">
         <f aca="false">SUBSTITUTE(LOWER(SUBSTITUTE(SUBSTITUTE(C37, "(", ""), ")", "")), " ", "_")</f>
         <v>implants_1_rod</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B38" s="0" t="str">
         <f aca="false">SUBSTITUTE(LOWER(SUBSTITUTE(SUBSTITUTE(C38, "(", ""), ")", "")), " ", "_")</f>
         <v>implants_2_rods</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B39" s="0" t="str">
         <f aca="false">SUBSTITUTE(LOWER(SUBSTITUTE(SUBSTITUTE(C39, "(", ""), ")", "")), " ", "_")</f>
         <v>iud</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B40" s="0" t="str">
         <f aca="false">SUBSTITUTE(LOWER(SUBSTITUTE(SUBSTITUTE(C40, "(", ""), ")", "")), " ", "_")</f>
         <v>condoms</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B41" s="0" t="str">
         <f aca="false">SUBSTITUTE(LOWER(SUBSTITUTE(SUBSTITUTE(C41, "(", ""), ")", "")), " ", "_")</f>
         <v>tubal_ligation</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B42" s="0" t="str">
         <f aca="false">SUBSTITUTE(LOWER(SUBSTITUTE(SUBSTITUTE(C42, "(", ""), ")", "")), " ", "_")</f>
         <v>cycle_beads</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6869,26 +6885,26 @@
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="B45" s="0" t="str">
         <f aca="false">SUBSTITUTE(LOWER(SUBSTITUTE(SUBSTITUTE(C45, "(", ""), ")", "")), " ", "_")</f>
         <v>wants_to_get_pregnant</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="B46" s="0" t="str">
         <f aca="false">SUBSTITUTE(LOWER(SUBSTITUTE(SUBSTITUTE(C46, "(", ""), ")", "")), " ", "_")</f>
         <v>did_not_want_fp</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6899,13 +6915,13 @@
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="29" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B48" s="29" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="C48" s="29" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="D48" s="29"/>
       <c r="E48" s="29"/>
@@ -6930,13 +6946,13 @@
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="29" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B49" s="29" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="C49" s="29" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="D49" s="29"/>
       <c r="E49" s="29"/>
@@ -6962,226 +6978,226 @@
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="29" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B58" s="29" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="C58" s="29" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="29" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B59" s="29" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="C59" s="29" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="29" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B60" s="29" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="C60" s="29" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="29" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B61" s="29" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C61" s="29" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="28" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="B63" s="28" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="C63" s="29" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="28" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="B64" s="28" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C64" s="29" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="28" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="B65" s="28" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="C65" s="29" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="28" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="B66" s="28" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="C66" s="29" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="28" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="B67" s="28" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C67" s="29" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="C72" s="34" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>